<commit_message>
Updated to more accurate RU translations
Signed-off-by: Leanid Astrakou <lastrakou@rocketsoftware.com>
</commit_message>
<xml_diff>
--- a/Translation/Zowe Virtual Desktop Translation Reference.xlsx
+++ b/Translation/Zowe Virtual Desktop Translation Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rocketsoftwareinc-my.sharepoint.com/personal/jlinardon_rocketsoftware_com/Documents/ZOWE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lastrakou\Desktop\zlux\community\Translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{DC55E723-C124-41DB-8842-C7E7CD492C56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{10337467-01F5-4FDF-9DB6-39BFA183F3F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0F7921-0685-422F-A45E-F7325039E7A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Constructs" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="1338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="1339">
   <si>
     <t>Zowe Virtual Desktop Translation Reference</t>
   </si>
@@ -3776,12 +3776,6 @@
     <t>无法找到对应ID的应用</t>
   </si>
   <si>
-    <t>Тип программы</t>
-  </si>
-  <si>
-    <t>Версия программы</t>
-  </si>
-  <si>
     <t>Закрыть все</t>
   </si>
   <si>
@@ -4065,6 +4059,15 @@
   </si>
   <si>
     <t>错误 保存变量</t>
+  </si>
+  <si>
+    <t>Приложение</t>
+  </si>
+  <si>
+    <t>Тип приложение</t>
+  </si>
+  <si>
+    <t>Версия приложение</t>
   </si>
 </sst>
 </file>
@@ -4680,9 +4683,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -4884,7 +4887,7 @@
         <v>59</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>1241</v>
+        <v>1337</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>60</v>
@@ -4928,7 +4931,7 @@
         <v>77</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>1242</v>
+        <v>1338</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>80</v>
@@ -4972,7 +4975,7 @@
         <v>88</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>89</v>
+        <v>1336</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>87</v>
@@ -5554,7 +5557,7 @@
         <v>240</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>241</v>
@@ -5756,22 +5759,22 @@
         <v>93</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -6270,22 +6273,22 @@
         <v>93</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="D46" s="26" t="s">
         <v>234</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -7522,7 +7525,7 @@
         <v>85</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="F81" s="15" t="s">
         <v>97</v>
@@ -7566,7 +7569,7 @@
         <v>173</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="F82" s="15" t="s">
         <v>174</v>
@@ -7636,7 +7639,7 @@
         <v>548</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="F84" s="15" t="s">
         <v>550</v>
@@ -8046,7 +8049,7 @@
         <v>697</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="F98" s="15" t="s">
         <v>698</v>
@@ -9114,7 +9117,7 @@
         <v>202</v>
       </c>
       <c r="E128" s="16" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="F128" s="15" t="s">
         <v>205</v>
@@ -9158,7 +9161,7 @@
         <v>217</v>
       </c>
       <c r="E129" s="16" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="F129" s="15" t="s">
         <v>218</v>
@@ -9238,19 +9241,19 @@
         <v>93</v>
       </c>
       <c r="C131" s="29" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="D131" s="26" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="E131" s="30" t="s">
         <v>825</v>
       </c>
       <c r="F131" s="15" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="G131" s="26" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="H131" s="26" t="s">
         <v>804</v>
@@ -14545,7 +14548,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -14634,7 +14637,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="D12" s="4"/>
     </row>
@@ -14989,7 +14992,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
@@ -15000,7 +15003,7 @@
         <v>8</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
@@ -15011,7 +15014,7 @@
         <v>9</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
@@ -15022,7 +15025,7 @@
         <v>10</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
@@ -15044,7 +15047,7 @@
         <v>14</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
@@ -15055,7 +15058,7 @@
         <v>7</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
@@ -15066,7 +15069,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
@@ -15077,7 +15080,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
@@ -15088,7 +15091,7 @@
         <v>10</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
@@ -15099,7 +15102,7 @@
         <v>12</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
@@ -15110,7 +15113,7 @@
         <v>14</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
@@ -15121,7 +15124,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
@@ -15132,7 +15135,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
@@ -15143,7 +15146,7 @@
         <v>9</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1">
@@ -15154,7 +15157,7 @@
         <v>10</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
@@ -15165,7 +15168,7 @@
         <v>12</v>
       </c>
       <c r="C56" s="26" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1">
@@ -15176,7 +15179,7 @@
         <v>14</v>
       </c>
       <c r="C57" s="26" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1">
@@ -15187,7 +15190,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
@@ -15198,7 +15201,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="26" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1">
@@ -15209,7 +15212,7 @@
         <v>9</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1">
@@ -15220,7 +15223,7 @@
         <v>10</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
@@ -15231,7 +15234,7 @@
         <v>12</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
@@ -15242,7 +15245,7 @@
         <v>14</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
@@ -15253,7 +15256,7 @@
         <v>7</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
@@ -15264,7 +15267,7 @@
         <v>8</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
@@ -15275,7 +15278,7 @@
         <v>9</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
@@ -15286,7 +15289,7 @@
         <v>10</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
@@ -15297,7 +15300,7 @@
         <v>12</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1">
@@ -15308,7 +15311,7 @@
         <v>14</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
@@ -15319,7 +15322,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1">
@@ -15330,7 +15333,7 @@
         <v>8</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1">
@@ -15341,7 +15344,7 @@
         <v>9</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1">
@@ -15352,7 +15355,7 @@
         <v>10</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1">
@@ -15363,7 +15366,7 @@
         <v>12</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
@@ -15374,7 +15377,7 @@
         <v>14</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1">
@@ -18393,7 +18396,7 @@
         <v>85</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>97</v>
@@ -18416,7 +18419,7 @@
         <v>173</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>174</v>
@@ -18462,7 +18465,7 @@
         <v>202</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>205</v>
@@ -18485,7 +18488,7 @@
         <v>217</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>218</v>
@@ -19516,7 +19519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
@@ -19584,7 +19587,7 @@
         <v>502</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>503</v>
@@ -19630,7 +19633,7 @@
         <v>515</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>516</v>
@@ -19653,7 +19656,7 @@
         <v>520</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>521</v>
@@ -19676,7 +19679,7 @@
         <v>525</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>526</v>
@@ -19699,7 +19702,7 @@
         <v>530</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>531</v>
@@ -19745,7 +19748,7 @@
         <v>539</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>542</v>
@@ -19768,7 +19771,7 @@
         <v>549</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>553</v>
@@ -19791,7 +19794,7 @@
         <v>558</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>559</v>
@@ -19814,7 +19817,7 @@
         <v>563</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>564</v>
@@ -19929,7 +19932,7 @@
         <v>584</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>586</v>
@@ -19994,7 +19997,7 @@
         <v>610</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>613</v>
@@ -20040,7 +20043,7 @@
         <v>626</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>629</v>
@@ -20063,7 +20066,7 @@
         <v>636</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>639</v>
@@ -20086,7 +20089,7 @@
         <v>650</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>651</v>
@@ -20132,7 +20135,7 @@
         <v>1235</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>1230</v>
@@ -20155,7 +20158,7 @@
         <v>1236</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>1229</v>
@@ -20178,7 +20181,7 @@
         <v>1237</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>1231</v>
@@ -20195,22 +20198,22 @@
         <v>13</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="14.25" customHeight="1">
@@ -20218,22 +20221,22 @@
         <v>13</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1">
@@ -20241,22 +20244,22 @@
         <v>13</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1"/>

</xml_diff>